<commit_message>
Update packages, add interventions in isolation
</commit_message>
<xml_diff>
--- a/applications/Susceptibility/outbreak/policy_packages.xlsx
+++ b/applications/Susceptibility/outbreak/policy_packages.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\covid\covasim-australia\applications\Susceptibility\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\covid\covasim-australia\applications\Susceptibility\outbreak\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28CB2C18-C24A-4614-B2A3-807CF219936A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D80C41BD-B2B3-4C72-9A27-5DCA7C3AC237}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="870" yWindow="3510" windowWidth="32325" windowHeight="11640" xr2:uid="{363A7447-5636-4312-8C61-443E964E1E89}"/>
+    <workbookView xWindow="10320" yWindow="1740" windowWidth="26760" windowHeight="12885" xr2:uid="{363A7447-5636-4312-8C61-443E964E1E89}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="65">
   <si>
     <t>lockdown</t>
   </si>
@@ -138,40 +138,94 @@
     <t>Relax 5</t>
   </si>
   <si>
-    <t>Relax 6</t>
-  </si>
-  <si>
     <t>No policies</t>
   </si>
   <si>
-    <t>NL Full lockdown</t>
-  </si>
-  <si>
-    <t>NL Relax 1</t>
-  </si>
-  <si>
-    <t>NL Relax 2</t>
-  </si>
-  <si>
-    <t>NL Relax 3</t>
-  </si>
-  <si>
-    <t>NL Relax 4</t>
-  </si>
-  <si>
-    <t>NL Relax 5</t>
-  </si>
-  <si>
-    <t>NL Relax 6</t>
-  </si>
-  <si>
-    <t>NL Pre outbreak</t>
-  </si>
-  <si>
-    <t>NL Distancing only</t>
-  </si>
-  <si>
     <t>lockdown_relax</t>
+  </si>
+  <si>
+    <t>Relaxed lockdown</t>
+  </si>
+  <si>
+    <t>Economic</t>
+  </si>
+  <si>
+    <t>p_lockdown</t>
+  </si>
+  <si>
+    <t>p_lockdown_relax</t>
+  </si>
+  <si>
+    <t>p_beach0</t>
+  </si>
+  <si>
+    <t>p_beach2</t>
+  </si>
+  <si>
+    <t>p_beach10</t>
+  </si>
+  <si>
+    <t>p_nat_parks0</t>
+  </si>
+  <si>
+    <t>p_church0</t>
+  </si>
+  <si>
+    <t>p_church_4sqm</t>
+  </si>
+  <si>
+    <t>p_cafe_restaurant0</t>
+  </si>
+  <si>
+    <t>p_cafe_restaurant_4sqm</t>
+  </si>
+  <si>
+    <t>p_pub_bar0</t>
+  </si>
+  <si>
+    <t>p_pub_bar_4sqm</t>
+  </si>
+  <si>
+    <t>p_outdoor2</t>
+  </si>
+  <si>
+    <t>p_outdoor10</t>
+  </si>
+  <si>
+    <t>p_outdoor200</t>
+  </si>
+  <si>
+    <t>p_pSports</t>
+  </si>
+  <si>
+    <t>p_cSports</t>
+  </si>
+  <si>
+    <t>p_child_care</t>
+  </si>
+  <si>
+    <t>p_schools</t>
+  </si>
+  <si>
+    <t>p_retail</t>
+  </si>
+  <si>
+    <t>p_entertainment</t>
+  </si>
+  <si>
+    <t>p_large_events</t>
+  </si>
+  <si>
+    <t>p_NE_work</t>
+  </si>
+  <si>
+    <t>p_NE_health</t>
+  </si>
+  <si>
+    <t>p_social</t>
+  </si>
+  <si>
+    <t>p_isolate_aged_care</t>
   </si>
 </sst>
 </file>
@@ -532,27 +586,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AFDE838-72F0-469D-A110-71C7430CE35C}">
-  <dimension ref="A1:T27"/>
+  <dimension ref="A1:AM28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="V17" sqref="V17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.28515625" customWidth="1"/>
     <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="18" width="10" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="16" width="10" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
@@ -560,22 +614,22 @@
         <v>27</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>28</v>
@@ -584,101 +638,138 @@
         <v>29</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AM1" s="1"/>
+    </row>
+    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>26</v>
       </c>
-      <c r="C2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" t="s">
-        <v>26</v>
-      </c>
-      <c r="J2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="M2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>36</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" t="s">
+        <v>26</v>
       </c>
       <c r="L3" t="s">
         <v>26</v>
       </c>
-      <c r="M3" t="s">
-        <v>26</v>
-      </c>
       <c r="N3" t="s">
         <v>26</v>
       </c>
-      <c r="O3" t="s">
-        <v>26</v>
-      </c>
-      <c r="P3" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>26</v>
-      </c>
-      <c r="R3" t="s">
-        <v>26</v>
-      </c>
-      <c r="S3" t="s">
-        <v>26</v>
-      </c>
-      <c r="T3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -691,39 +782,33 @@
       <c r="D4" t="s">
         <v>26</v>
       </c>
-      <c r="L4" t="s">
-        <v>26</v>
-      </c>
-      <c r="M4" t="s">
-        <v>26</v>
-      </c>
-      <c r="N4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="O4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="E5" t="s">
         <v>26</v>
       </c>
-      <c r="O5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="P5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="F6" t="s">
         <v>26</v>
       </c>
-      <c r="P6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="Q6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -748,29 +833,11 @@
       <c r="H7" t="s">
         <v>26</v>
       </c>
-      <c r="L7" t="s">
-        <v>26</v>
-      </c>
-      <c r="M7" t="s">
-        <v>26</v>
-      </c>
-      <c r="N7" t="s">
-        <v>26</v>
-      </c>
-      <c r="O7" t="s">
-        <v>26</v>
-      </c>
-      <c r="P7" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>26</v>
-      </c>
       <c r="R7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -786,31 +853,28 @@
       <c r="E8" t="s">
         <v>26</v>
       </c>
-      <c r="L8" t="s">
-        <v>26</v>
-      </c>
-      <c r="M8" t="s">
-        <v>26</v>
-      </c>
-      <c r="N8" t="s">
-        <v>26</v>
-      </c>
-      <c r="O8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="S8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="F9" t="s">
         <v>26</v>
       </c>
-      <c r="P9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L9" t="s">
+        <v>26</v>
+      </c>
+      <c r="T9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -823,17 +887,11 @@
       <c r="D10" t="s">
         <v>26</v>
       </c>
-      <c r="L10" t="s">
-        <v>26</v>
-      </c>
-      <c r="M10" t="s">
-        <v>26</v>
-      </c>
-      <c r="N10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -843,14 +901,17 @@
       <c r="F11" t="s">
         <v>26</v>
       </c>
-      <c r="O11" t="s">
-        <v>26</v>
-      </c>
-      <c r="P11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I11" t="s">
+        <v>26</v>
+      </c>
+      <c r="L11" t="s">
+        <v>26</v>
+      </c>
+      <c r="V11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -863,17 +924,11 @@
       <c r="D12" t="s">
         <v>26</v>
       </c>
-      <c r="L12" t="s">
-        <v>26</v>
-      </c>
-      <c r="M12" t="s">
-        <v>26</v>
-      </c>
-      <c r="N12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -889,20 +944,17 @@
       <c r="H13" t="s">
         <v>26</v>
       </c>
-      <c r="O13" t="s">
-        <v>26</v>
-      </c>
-      <c r="P13" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>26</v>
-      </c>
-      <c r="R13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I13" t="s">
+        <v>26</v>
+      </c>
+      <c r="L13" t="s">
+        <v>26</v>
+      </c>
+      <c r="X13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -915,17 +967,11 @@
       <c r="D14" t="s">
         <v>26</v>
       </c>
-      <c r="L14" t="s">
-        <v>26</v>
-      </c>
-      <c r="M14" t="s">
-        <v>26</v>
-      </c>
-      <c r="N14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="Y14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -941,25 +987,25 @@
       <c r="H15" t="s">
         <v>26</v>
       </c>
-      <c r="O15" t="s">
-        <v>26</v>
-      </c>
-      <c r="P15" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>26</v>
-      </c>
-      <c r="R15" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="L15" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="I16" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -987,26 +1033,11 @@
       <c r="L17" t="s">
         <v>26</v>
       </c>
-      <c r="M17" t="s">
-        <v>26</v>
-      </c>
-      <c r="N17" t="s">
-        <v>26</v>
-      </c>
-      <c r="O17" t="s">
-        <v>26</v>
-      </c>
-      <c r="P17" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>26</v>
-      </c>
-      <c r="R17" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="AB17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -1025,17 +1056,11 @@
       <c r="L18" t="s">
         <v>26</v>
       </c>
-      <c r="M18" t="s">
-        <v>26</v>
-      </c>
-      <c r="N18" t="s">
-        <v>26</v>
-      </c>
-      <c r="O18" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="AC18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -1060,29 +1085,11 @@
       <c r="H19" t="s">
         <v>26</v>
       </c>
-      <c r="L19" t="s">
-        <v>26</v>
-      </c>
-      <c r="M19" t="s">
-        <v>26</v>
-      </c>
-      <c r="N19" t="s">
-        <v>26</v>
-      </c>
-      <c r="O19" t="s">
-        <v>26</v>
-      </c>
-      <c r="P19" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>26</v>
-      </c>
-      <c r="R19" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="AD19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -1092,14 +1099,11 @@
       <c r="C20" t="s">
         <v>26</v>
       </c>
-      <c r="L20" t="s">
-        <v>26</v>
-      </c>
-      <c r="M20" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="AE20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -1124,29 +1128,11 @@
       <c r="H21" t="s">
         <v>26</v>
       </c>
-      <c r="L21" t="s">
-        <v>26</v>
-      </c>
-      <c r="M21" t="s">
-        <v>26</v>
-      </c>
-      <c r="N21" t="s">
-        <v>26</v>
-      </c>
-      <c r="O21" t="s">
-        <v>26</v>
-      </c>
-      <c r="P21" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>26</v>
-      </c>
-      <c r="R21" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="AF21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -1171,29 +1157,11 @@
       <c r="H22" t="s">
         <v>26</v>
       </c>
-      <c r="L22" t="s">
-        <v>26</v>
-      </c>
-      <c r="M22" t="s">
-        <v>26</v>
-      </c>
-      <c r="N22" t="s">
-        <v>26</v>
-      </c>
-      <c r="O22" t="s">
-        <v>26</v>
-      </c>
-      <c r="P22" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>26</v>
-      </c>
-      <c r="R22" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="AG22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -1224,29 +1192,11 @@
       <c r="L23" t="s">
         <v>26</v>
       </c>
-      <c r="M23" t="s">
-        <v>26</v>
-      </c>
-      <c r="N23" t="s">
-        <v>26</v>
-      </c>
-      <c r="O23" t="s">
-        <v>26</v>
-      </c>
-      <c r="P23" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>26</v>
-      </c>
-      <c r="R23" t="s">
-        <v>26</v>
-      </c>
-      <c r="S23" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="AH23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -1271,29 +1221,11 @@
       <c r="H24" t="s">
         <v>26</v>
       </c>
-      <c r="L24" t="s">
-        <v>26</v>
-      </c>
-      <c r="M24" t="s">
-        <v>26</v>
-      </c>
-      <c r="N24" t="s">
-        <v>26</v>
-      </c>
-      <c r="O24" t="s">
-        <v>26</v>
-      </c>
-      <c r="P24" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>26</v>
-      </c>
-      <c r="R24" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="AI24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -1318,40 +1250,25 @@
       <c r="H25" t="s">
         <v>26</v>
       </c>
-      <c r="L25" t="s">
-        <v>26</v>
-      </c>
-      <c r="M25" t="s">
-        <v>26</v>
-      </c>
-      <c r="N25" t="s">
-        <v>26</v>
-      </c>
-      <c r="O25" t="s">
-        <v>26</v>
-      </c>
-      <c r="P25" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q25" t="s">
-        <v>26</v>
-      </c>
-      <c r="R25" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="AJ25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>23</v>
       </c>
       <c r="B26" t="s">
         <v>26</v>
       </c>
-      <c r="L26" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>26</v>
+      </c>
+      <c r="AK26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>24</v>
       </c>
@@ -1379,22 +1296,12 @@
       <c r="L27" t="s">
         <v>26</v>
       </c>
-      <c r="M27" t="s">
-        <v>26</v>
-      </c>
-      <c r="N27" t="s">
-        <v>26</v>
-      </c>
-      <c r="O27" t="s">
-        <v>26</v>
-      </c>
-      <c r="P27" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>26</v>
-      </c>
-      <c r="R27" t="s">
+      <c r="AL27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AM28" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>